<commit_message>
Updated link on schedule page.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jb2329/Dropbox (Personal)/School/Teaching/EPSY630 2020 Spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90111A96-E4AB-5145-837D-3A34C7006FE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD5B910-5D17-5543-BEDD-3AA1F532F770}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4840" yWindow="4540" windowWidth="28800" windowHeight="17540" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
     <t>[Intro Course Slides](/slides/01-Intro_to_Course.html), [Intro R Slides](/slides/02-IntroR.html)</t>
   </si>
   <si>
-    <t>Diez, et al Chapter 5&lt;br/&gt;[Survey Results](/slides/2020-02-03-Survey_Results.html), [Slides](/2020-02-03-Foundation_for_Inference.html)</t>
+    <t>Diez, et al Chapter 5&lt;br/&gt;[Survey Results](/slides/2020-02-03-Survey_Results.html), [Slides](/slides/2020-02-03-Foundation_for_Inference.html)</t>
   </si>
 </sst>
 </file>

</xml_diff>